<commit_message>
expanded date column in excel sheet
expanded date column
</commit_message>
<xml_diff>
--- a/Data/Western_Snowy_Plover_Window_Survey_dataset.xlsx
+++ b/Data/Western_Snowy_Plover_Window_Survey_dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jacob_cochran_fws_gov/Documents/Desktop/R Markdown - Quarto Workshops/2025 Virtual Course/Quarto_Exercise-2025_Data_Management_Workshop/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jason_ross_fws_gov/Documents/Documents/GitHub/Quarto_Exercise-2025_Data_Management_Workshop/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="11_D988C6ACEA9225991F964136A7A82AC7A8F6DA74" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{834DF642-81F8-4316-83FA-1A53F331368F}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="11_D988C6ACEA9225991F964136A7A82AC7A8F6DA74" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0870C99C-CE5F-4CD4-9232-06AFD79E07FD}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="12960" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observation Data_0" sheetId="2" r:id="rId1"/>
@@ -1677,25 +1677,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.47265625" customWidth="1"/>
-    <col min="2" max="2" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.68359375" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1727,7 +1726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>424</v>
       </c>
@@ -1760,7 +1759,7 @@
         <v>-124.06047725568401</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>424</v>
       </c>
@@ -1793,7 +1792,7 @@
         <v>-124.07804882188201</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>424</v>
       </c>
@@ -1826,7 +1825,7 @@
         <v>-124.08259582902799</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>424</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>-124.124318158489</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>424</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>-124.125059260821</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1925,7 +1924,7 @@
         <v>-124.061751776261</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1958,7 +1957,7 @@
         <v>-124.069624662384</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>-124.061452056091</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2024,7 +2023,7 @@
         <v>-124.059563751685</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2057,7 +2056,7 @@
         <v>-124.08021406345</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>424</v>
       </c>
@@ -2090,7 +2089,7 @@
         <v>-124.12832379475699</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>424</v>
       </c>
@@ -2123,7 +2122,7 @@
         <v>-124.1313583676</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>424</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>-124.129962464111</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>424</v>
       </c>
@@ -2189,7 +2188,7 @@
         <v>-124.1313583676</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>424</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>-124.344705275519</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2255,7 +2254,7 @@
         <v>-124.324903605872</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2288,7 +2287,7 @@
         <v>-124.324087042226</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2321,7 +2320,7 @@
         <v>-124.442904730173</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -2354,7 +2353,7 @@
         <v>-124.442513686098</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2387,7 +2386,7 @@
         <v>-124.44517005041099</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>424</v>
       </c>
@@ -2420,7 +2419,7 @@
         <v>-124.11331446049699</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>424</v>
       </c>
@@ -2453,7 +2452,7 @@
         <v>-124.114600467636</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>424</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>-124.355847107801</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>424</v>
       </c>
@@ -2519,7 +2518,7 @@
         <v>-124.35431121405701</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>424</v>
       </c>
@@ -2552,7 +2551,7 @@
         <v>-124.354731785903</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2585,7 +2584,7 @@
         <v>-124.110940057512</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2618,7 +2617,7 @@
         <v>-124.113764562995</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2651,7 +2650,7 @@
         <v>-124.114278965851</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2684,7 +2683,7 @@
         <v>-124.35623220430899</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2731,9 +2730,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2762,7 +2761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2785,7 +2784,7 @@
         <v>44.746283698680202</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>44.652628811044799</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2831,7 +2830,7 @@
         <v>44.424496639712999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2854,7 +2853,7 @@
         <v>44.437084280937498</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2877,7 +2876,7 @@
         <v>42.005093163773502</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2900,7 +2899,7 @@
         <v>41.998466626617798</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2923,7 +2922,7 @@
         <v>44.400479492926301</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2946,7 +2945,7 @@
         <v>44.420414923080202</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>45.703507775190403</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>45.668525849692401</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3015,7 +3014,7 @@
         <v>43.790044895542003</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3038,7 +3037,7 @@
         <v>43.672720325273303</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3061,7 +3060,7 @@
         <v>42.461773519151997</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3084,7 +3083,7 @@
         <v>42.4231421689882</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3107,7 +3106,7 @@
         <v>44.436483557864499</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3130,7 +3129,7 @@
         <v>44.424961357090901</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>44.452539996454703</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3176,7 +3175,7 @@
         <v>44.47804</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>44.452640453478502</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>44.426049905304403</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3245,7 +3244,7 @@
         <v>44.621709753598999</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3268,7 +3267,7 @@
         <v>44.625478587275801</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3291,7 +3290,7 @@
         <v>46.722872280625197</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3314,7 +3313,7 @@
         <v>46.706706512243002</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3337,7 +3336,7 @@
         <v>46.849187616400997</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3360,7 +3359,7 @@
         <v>46.737381596195398</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3383,7 +3382,7 @@
         <v>46.962825917194799</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3406,7 +3405,7 @@
         <v>47.070339628980001</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3429,7 +3428,7 @@
         <v>47.070376414277298</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3452,7 +3451,7 @@
         <v>47.139650291148698</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>47.1223990197281</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3498,7 +3497,7 @@
         <v>47.139988043207502</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3521,7 +3520,7 @@
         <v>46.945512664039001</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3544,7 +3543,7 @@
         <v>46.940318976574602</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3567,7 +3566,7 @@
         <v>44.920036541722503</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3590,7 +3589,7 @@
         <v>44.923847750348699</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3613,7 +3612,7 @@
         <v>43.185445866953302</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3636,7 +3635,7 @@
         <v>43.127067340500801</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3665,7 +3664,7 @@
         <v>45.268939733837698</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3694,7 +3693,7 @@
         <v>45.287624807543096</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3717,7 +3716,7 @@
         <v>43.893166577385898</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3740,7 +3739,7 @@
         <v>44.015011653121398</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3763,7 +3762,7 @@
         <v>45.192489090852099</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3786,7 +3785,7 @@
         <v>45.161599290678602</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3809,7 +3808,7 @@
         <v>46.228550830989803</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3832,7 +3831,7 @@
         <v>46.237270266310396</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3855,7 +3854,7 @@
         <v>46.27111</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3878,7 +3877,7 @@
         <v>46.296759999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3907,7 +3906,7 @@
         <v>46.30292</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3936,7 +3935,7 @@
         <v>46.548409999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3965,7 +3964,7 @@
         <v>46.548409999999997</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>46.662190000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4017,7 +4016,7 @@
         <v>46.012303934484997</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4040,7 +4039,7 @@
         <v>46.023667131546603</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4063,7 +4062,7 @@
         <v>42.988783938248297</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4086,7 +4085,7 @@
         <v>42.894779999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4109,7 +4108,7 @@
         <v>43.0726623894083</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4132,7 +4131,7 @@
         <v>42.991270145476001</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4155,7 +4154,7 @@
         <v>43.412842286147701</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4178,7 +4177,7 @@
         <v>43.358952405587203</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4201,7 +4200,7 @@
         <v>43.576115693071998</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4224,7 +4223,7 @@
         <v>43.555147141559097</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4247,7 +4246,7 @@
         <v>43.6320663862857</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4270,7 +4269,7 @@
         <v>43.577572230854301</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4293,7 +4292,7 @@
         <v>43.806248332874397</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4316,7 +4315,7 @@
         <v>43.790289767927497</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4339,7 +4338,7 @@
         <v>43.8689014508996</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4362,7 +4361,7 @@
         <v>43.808626890425998</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4385,7 +4384,7 @@
         <v>43.924149093498997</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4408,7 +4407,7 @@
         <v>43.870535004871201</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4431,7 +4430,7 @@
         <v>44.088894938977198</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4454,7 +4453,7 @@
         <v>44.052713474780397</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4477,7 +4476,7 @@
         <v>45.5057841</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4500,7 +4499,7 @@
         <v>45.530504800000003</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4523,7 +4522,7 @@
         <v>44.612520098828803</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4546,7 +4545,7 @@
         <v>44.598199772947503</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4569,7 +4568,7 @@
         <v>42.275698142188901</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4592,7 +4591,7 @@
         <v>42.271664597405596</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4615,7 +4614,7 @@
         <v>45.369753550225603</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4638,7 +4637,7 @@
         <v>45.428818912750103</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4661,7 +4660,7 @@
         <v>45.528397535397502</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4684,7 +4683,7 @@
         <v>45.565469980874099</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4707,7 +4706,7 @@
         <v>46.113855582881499</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4730,7 +4729,7 @@
         <v>46.1497784413137</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4753,7 +4752,7 @@
         <v>42.561232500985597</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4776,7 +4775,7 @@
         <v>42.536371333628203</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4799,7 +4798,7 @@
         <v>42.871349484528999</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4822,7 +4821,7 @@
         <v>42.854463323981797</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4845,7 +4844,7 @@
         <v>44.057534133786802</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4868,7 +4867,7 @@
         <v>44.018805982570001</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4891,7 +4890,7 @@
         <v>42.791427929488897</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4914,7 +4913,7 @@
         <v>42.813695513709803</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4937,7 +4936,7 @@
         <v>42.824415598925498</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4960,7 +4959,7 @@
         <v>42.813543384211798</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4983,7 +4982,7 @@
         <v>44.597141656258501</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5006,7 +5005,7 @@
         <v>44.612760404593402</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>99</v>
       </c>
@@ -5029,7 +5028,7 @@
         <v>44.620675014887397</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>100</v>
       </c>
@@ -5052,7 +5051,7 @@
         <v>44.626081399382201</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>101</v>
       </c>
@@ -5075,7 +5074,7 @@
         <v>44.4006690005331</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>102</v>
       </c>
@@ -5098,7 +5097,7 @@
         <v>44.4198204416181</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>103</v>
       </c>
@@ -5121,7 +5120,7 @@
         <v>44.423557625675201</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>104</v>
       </c>
@@ -5144,7 +5143,7 @@
         <v>44.483085075744398</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>105</v>
       </c>
@@ -5167,7 +5166,7 @@
         <v>42.560674170748598</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>106</v>
       </c>
@@ -5190,7 +5189,7 @@
         <v>42.5364919842212</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>107</v>
       </c>
@@ -5213,7 +5212,7 @@
         <v>45.201974459146697</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>108</v>
       </c>
@@ -5236,7 +5235,7 @@
         <v>45.161236089665401</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>109</v>
       </c>
@@ -5259,7 +5258,7 @@
         <v>42.869024863669097</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>110</v>
       </c>
@@ -5282,7 +5281,7 @@
         <v>42.851660299977503</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>111</v>
       </c>
@@ -5305,7 +5304,7 @@
         <v>43.210875055151497</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>112</v>
       </c>
@@ -5328,7 +5327,7 @@
         <v>43.125684601347203</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>113</v>
       </c>
@@ -5351,7 +5350,7 @@
         <v>45.531289676437702</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>114</v>
       </c>
@@ -5374,7 +5373,7 @@
         <v>45.5656848021926</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>115</v>
       </c>
@@ -5397,7 +5396,7 @@
         <v>44.658294120119997</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>116</v>
       </c>
@@ -5420,7 +5419,7 @@
         <v>44.673872092350202</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>117</v>
       </c>
@@ -5443,7 +5442,7 @@
         <v>41.999269581707601</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>118</v>
       </c>
@@ -5466,7 +5465,7 @@
         <v>42.004999644039103</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>119</v>
       </c>
@@ -5489,7 +5488,7 @@
         <v>42.301015774601701</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>120</v>
       </c>
@@ -5512,7 +5511,7 @@
         <v>42.287029961477799</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>121</v>
       </c>
@@ -5535,7 +5534,7 @@
         <v>42.461599833126598</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>122</v>
       </c>
@@ -5558,7 +5557,7 @@
         <v>42.422917579963197</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>123</v>
       </c>
@@ -5581,7 +5580,7 @@
         <v>46.235981258283203</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>124</v>
       </c>
@@ -5604,7 +5603,7 @@
         <v>46.229201757936302</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>125</v>
       </c>
@@ -5627,7 +5626,7 @@
         <v>45.034729292883597</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>126</v>
       </c>
@@ -5650,7 +5649,7 @@
         <v>45.039607994372503</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>127</v>
       </c>
@@ -5673,7 +5672,7 @@
         <v>44.919619910038897</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>128</v>
       </c>
@@ -5696,7 +5695,7 @@
         <v>44.924675722654001</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>131</v>
       </c>
@@ -5719,7 +5718,7 @@
         <v>46.746428664774797</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>132</v>
       </c>
@@ -5742,7 +5741,7 @@
         <v>46.793963257569501</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>133</v>
       </c>
@@ -5765,7 +5764,7 @@
         <v>46.7239100385802</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>134</v>
       </c>
@@ -5788,7 +5787,7 @@
         <v>46.705886454818902</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>135</v>
       </c>
@@ -5811,7 +5810,7 @@
         <v>46.949323893341997</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>136</v>
       </c>
@@ -5834,7 +5833,7 @@
         <v>47.0703190822151</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>137</v>
       </c>
@@ -5857,7 +5856,7 @@
         <v>47.070269620757301</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>138</v>
       </c>
@@ -5880,7 +5879,7 @@
         <v>47.121056326509098</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>139</v>
       </c>
@@ -5903,7 +5902,7 @@
         <v>47.121304546928599</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>140</v>
       </c>
@@ -5926,7 +5925,7 @@
         <v>47.139862213588401</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>141</v>
       </c>
@@ -5949,7 +5948,7 @@
         <v>46.945399696498697</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>142</v>
       </c>
@@ -5972,7 +5971,7 @@
         <v>46.940997475119403</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>143</v>
       </c>
@@ -5995,7 +5994,7 @@
         <v>43.887672811539403</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>144</v>
       </c>
@@ -6018,7 +6017,7 @@
         <v>44.015505545641197</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>145</v>
       </c>
@@ -6041,7 +6040,7 @@
         <v>46.015113602977202</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>146</v>
       </c>
@@ -6064,7 +6063,7 @@
         <v>46.030820386381201</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>147</v>
       </c>
@@ -6087,7 +6086,7 @@
         <v>45.505717446212401</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>148</v>
       </c>
@@ -6110,7 +6109,7 @@
         <v>45.52761843671</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>149</v>
       </c>
@@ -6133,7 +6132,7 @@
         <v>42.827059237719503</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>150</v>
       </c>
@@ -6156,7 +6155,7 @@
         <v>42.796978041846799</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>151</v>
       </c>
@@ -6179,7 +6178,7 @@
         <v>46.148940000000003</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>152</v>
       </c>
@@ -6202,7 +6201,7 @@
         <v>46.113597009072599</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>153</v>
       </c>
@@ -6225,7 +6224,7 @@
         <v>45.267330000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>154</v>
       </c>
@@ -6248,7 +6247,7 @@
         <v>45.275184000000003</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>155</v>
       </c>
@@ -6271,7 +6270,7 @@
         <v>45.686861999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>156</v>
       </c>
@@ -6294,7 +6293,7 @@
         <v>45.657623000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>157</v>
       </c>
@@ -6317,7 +6316,7 @@
         <v>45.368820999999997</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>158</v>
       </c>
@@ -6340,7 +6339,7 @@
         <v>45.428162999999998</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>161</v>
       </c>
@@ -6363,7 +6362,7 @@
         <v>46.548360000000002</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>162</v>
       </c>
@@ -6386,7 +6385,7 @@
         <v>46.644930000000002</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>163</v>
       </c>
@@ -6409,7 +6408,7 @@
         <v>46.270697874028897</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>164</v>
       </c>
@@ -6432,7 +6431,7 @@
         <v>46.296869999999998</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>165</v>
       </c>
@@ -6455,7 +6454,7 @@
         <v>46.548360000000002</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>166</v>
       </c>
@@ -6478,7 +6477,7 @@
         <v>46.302500000000002</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>167</v>
       </c>
@@ -6501,7 +6500,7 @@
         <v>45.281725633697597</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>168</v>
       </c>
@@ -6524,7 +6523,7 @@
         <v>45.287159338570703</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>169</v>
       </c>
@@ -6547,7 +6546,7 @@
         <v>44.051109346742699</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>170</v>
       </c>
@@ -6570,7 +6569,7 @@
         <v>44.018586893399899</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>171</v>
       </c>
@@ -6593,7 +6592,7 @@
         <v>43.4117686389718</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>172</v>
       </c>
@@ -6616,7 +6615,7 @@
         <v>43.357080314873201</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>173</v>
       </c>
@@ -6639,7 +6638,7 @@
         <v>43.078991717235503</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>174</v>
       </c>
@@ -6662,7 +6661,7 @@
         <v>42.987718723990099</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>175</v>
       </c>
@@ -6685,7 +6684,7 @@
         <v>42.985425787687703</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>176</v>
       </c>
@@ -6708,7 +6707,7 @@
         <v>42.9026562309745</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>177</v>
       </c>
@@ -6731,7 +6730,7 @@
         <v>44.104890588505803</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>178</v>
       </c>
@@ -6754,7 +6753,7 @@
         <v>44.051791199009003</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>179</v>
       </c>
@@ -6777,7 +6776,7 @@
         <v>43.791056618631799</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>180</v>
       </c>
@@ -6800,7 +6799,7 @@
         <v>43.748527412098099</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>181</v>
       </c>
@@ -6823,7 +6822,7 @@
         <v>43.881593700912497</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>182</v>
       </c>
@@ -6846,7 +6845,7 @@
         <v>43.860108852297699</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>183</v>
       </c>
@@ -6869,7 +6868,7 @@
         <v>43.860184559931703</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>184</v>
       </c>
@@ -6892,7 +6891,7 @@
         <v>43.816591375265297</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>185</v>
       </c>
@@ -6915,7 +6914,7 @@
         <v>43.816452360830397</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>186</v>
       </c>
@@ -6938,7 +6937,7 @@
         <v>43.790668108073497</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>187</v>
       </c>
@@ -6961,7 +6960,7 @@
         <v>43.6561337504574</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>188</v>
       </c>
@@ -6984,7 +6983,7 @@
         <v>43.549108079019298</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>189</v>
       </c>
@@ -7007,7 +7006,7 @@
         <v>43.664442834905202</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>190</v>
       </c>
@@ -7030,7 +7029,7 @@
         <v>43.3628999455197</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>191</v>
       </c>
@@ -7053,7 +7052,7 @@
         <v>34.056795690033702</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>192</v>
       </c>
@@ -7076,7 +7075,7 @@
         <v>34.057464187188501</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>193</v>
       </c>
@@ -7105,7 +7104,7 @@
         <v>46.271541167202898</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>194</v>
       </c>
@@ -7134,7 +7133,7 @@
         <v>46.296730076082603</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>195</v>
       </c>
@@ -7157,7 +7156,7 @@
         <v>44.9258324314047</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>196</v>
       </c>
@@ -7180,7 +7179,7 @@
         <v>44.919713258124098</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>197</v>
       </c>
@@ -7203,7 +7202,7 @@
         <v>45.375441745823899</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>198</v>
       </c>
@@ -7226,7 +7225,7 @@
         <v>45.433783742499401</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>199</v>
       </c>
@@ -7249,7 +7248,7 @@
         <v>44.452666053898596</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>200</v>
       </c>
@@ -7272,7 +7271,7 @@
         <v>44.424285546364601</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>201</v>
       </c>
@@ -7295,7 +7294,7 @@
         <v>44.400478568454901</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>202</v>
       </c>
@@ -7318,7 +7317,7 @@
         <v>44.419718651356902</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>203</v>
       </c>
@@ -7341,7 +7340,7 @@
         <v>45.703531689568401</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>204</v>
       </c>
@@ -7364,7 +7363,7 @@
         <v>45.658283464353097</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>205</v>
       </c>
@@ -7387,7 +7386,7 @@
         <v>43.897198899999999</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>206</v>
       </c>
@@ -7410,7 +7409,7 @@
         <v>44.015410000000003</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>207</v>
       </c>
@@ -7433,7 +7432,7 @@
         <v>45.503399856879099</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>208</v>
       </c>
@@ -7456,7 +7455,7 @@
         <v>45.565389222839698</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>209</v>
       </c>
@@ -7479,7 +7478,7 @@
         <v>42.461785281347296</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>210</v>
       </c>
@@ -7502,7 +7501,7 @@
         <v>42.4232142482917</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>211</v>
       </c>
@@ -7525,7 +7524,7 @@
         <v>44.019081033097102</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>212</v>
       </c>
@@ -7548,7 +7547,7 @@
         <v>44.034979867348802</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>213</v>
       </c>
@@ -7571,7 +7570,7 @@
         <v>41.998723799183303</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>214</v>
       </c>
@@ -7594,7 +7593,7 @@
         <v>42.004954996657801</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>215</v>
       </c>
@@ -7617,7 +7616,7 @@
         <v>42.8710238004576</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>216</v>
       </c>
@@ -7640,7 +7639,7 @@
         <v>42.854682271373797</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>217</v>
       </c>
@@ -7663,7 +7662,7 @@
         <v>42.536861768500302</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>218</v>
       </c>
@@ -7686,7 +7685,7 @@
         <v>42.564322939183498</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>219</v>
       </c>
@@ -7715,7 +7714,7 @@
         <v>46.302406871760503</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>220</v>
       </c>
@@ -7744,7 +7743,7 @@
         <v>46.548294205966698</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>221</v>
       </c>
@@ -7767,7 +7766,7 @@
         <v>43.210666423748599</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>222</v>
       </c>
@@ -7790,7 +7789,7 @@
         <v>43.124708152061402</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>223</v>
       </c>
@@ -7813,7 +7812,7 @@
         <v>46.016831699487099</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>224</v>
       </c>
@@ -7836,7 +7835,7 @@
         <v>46.031310806296503</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>225</v>
       </c>
@@ -7859,7 +7858,7 @@
         <v>44.625613645223197</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>226</v>
       </c>
@@ -7882,7 +7881,7 @@
         <v>44.618197069450197</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>227</v>
       </c>
@@ -7905,7 +7904,7 @@
         <v>46.236663853067697</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>228</v>
       </c>
@@ -7928,7 +7927,7 @@
         <v>46.228865544168002</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>229</v>
       </c>
@@ -7951,7 +7950,7 @@
         <v>45.039160000000003</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>230</v>
       </c>
@@ -7974,7 +7973,7 @@
         <v>45.034680000000002</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>231</v>
       </c>
@@ -7997,7 +7996,7 @@
         <v>44.611725295803197</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>232</v>
       </c>
@@ -8020,7 +8019,7 @@
         <v>44.591244527493103</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>233</v>
       </c>
@@ -8043,7 +8042,7 @@
         <v>44.088529819902099</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>234</v>
       </c>
@@ -8066,7 +8065,7 @@
         <v>44.053867491918602</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>235</v>
       </c>
@@ -8089,7 +8088,7 @@
         <v>43.792846358704203</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>236</v>
       </c>
@@ -8112,7 +8111,7 @@
         <v>43.816476767409803</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>237</v>
       </c>
@@ -8135,7 +8134,7 @@
         <v>43.816474887036698</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>238</v>
       </c>
@@ -8158,7 +8157,7 @@
         <v>43.860187706480403</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>239</v>
       </c>
@@ -8181,7 +8180,7 @@
         <v>43.860219342677198</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>240</v>
       </c>
@@ -8204,7 +8203,7 @@
         <v>43.889525032350299</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>241</v>
       </c>
@@ -8227,7 +8226,7 @@
         <v>43.578938805256399</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>242</v>
       </c>
@@ -8250,7 +8249,7 @@
         <v>43.631549727571098</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>243</v>
       </c>
@@ -8273,7 +8272,7 @@
         <v>43.579356224145897</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>244</v>
       </c>
@@ -8296,7 +8295,7 @@
         <v>43.553790999396398</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>245</v>
       </c>
@@ -8319,7 +8318,7 @@
         <v>43.073681490296899</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>246</v>
       </c>
@@ -8342,7 +8341,7 @@
         <v>43.022722192054196</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>247</v>
       </c>
@@ -8365,7 +8364,7 @@
         <v>43.0009971917573</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>248</v>
       </c>
@@ -8388,7 +8387,7 @@
         <v>42.902563495099898</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>249</v>
       </c>
@@ -8411,7 +8410,7 @@
         <v>43.410224997711602</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>250</v>
       </c>
@@ -8434,7 +8433,7 @@
         <v>43.357226969039203</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>251</v>
       </c>
@@ -8457,7 +8456,7 @@
         <v>43.790295814581299</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>252</v>
       </c>
@@ -8480,7 +8479,7 @@
         <v>43.672217397985399</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>253</v>
       </c>
@@ -8503,7 +8502,7 @@
         <v>43.535499999999999</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>254</v>
       </c>
@@ -8526,7 +8525,7 @@
         <v>43.438639999999999</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>255</v>
       </c>
@@ -8549,7 +8548,7 @@
         <v>46.727483648227903</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>256</v>
       </c>
@@ -8572,7 +8571,7 @@
         <v>46.705430991447201</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>257</v>
       </c>
@@ -8595,7 +8594,7 @@
         <v>46.841184479701901</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>258</v>
       </c>
@@ -8618,7 +8617,7 @@
         <v>46.744161691606401</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>259</v>
       </c>
@@ -8641,7 +8640,7 @@
         <v>47.139867168129399</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>260</v>
       </c>
@@ -8664,7 +8663,7 @@
         <v>47.070333696147898</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>261</v>
       </c>
@@ -8687,7 +8686,7 @@
         <v>47.070261096622701</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>262</v>
       </c>
@@ -8710,7 +8709,7 @@
         <v>46.967784376104802</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>263</v>
       </c>
@@ -8733,7 +8732,7 @@
         <v>47.121348295116697</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>264</v>
       </c>
@@ -8756,7 +8755,7 @@
         <v>47.139941634338001</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>265</v>
       </c>
@@ -8779,7 +8778,7 @@
         <v>46.150072068820798</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>266</v>
       </c>
@@ -8802,7 +8801,7 @@
         <v>46.113669999999999</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>267</v>
       </c>
@@ -8825,7 +8824,7 @@
         <v>42.7976477136855</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>268</v>
       </c>
@@ -8848,7 +8847,7 @@
         <v>42.828128490866</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>269</v>
       </c>
@@ -8871,7 +8870,7 @@
         <v>44.651850000000003</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>270</v>
       </c>
@@ -8894,7 +8893,7 @@
         <v>44.671300000000002</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>271</v>
       </c>
@@ -8917,7 +8916,7 @@
         <v>45.191949610170603</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>272</v>
       </c>
@@ -8940,7 +8939,7 @@
         <v>45.162494595390299</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>273</v>
       </c>
@@ -8963,7 +8962,7 @@
         <v>46.548409999999997</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>274</v>
       </c>
@@ -8986,7 +8985,7 @@
         <v>46.662770000000002</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>275</v>
       </c>
@@ -9009,7 +9008,7 @@
         <v>45.281361395256802</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>276</v>
       </c>
@@ -9032,7 +9031,7 @@
         <v>45.298455056328699</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>277</v>
       </c>
@@ -9055,7 +9054,7 @@
         <v>45.266653674435197</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>278</v>
       </c>

</xml_diff>